<commit_message>
Changes made to the Fanconi scripts
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FC9B15-2432-D546-B2B5-5BCE37B99810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098E86D7-A741-1F45-9BE8-5232B4043353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="12600" windowHeight="16940" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="224">
   <si>
     <t>FirstName</t>
   </si>
@@ -714,6 +714,12 @@
   </si>
   <si>
     <t>ProxyLastName</t>
+  </si>
+  <si>
+    <t>Study Contact3</t>
+  </si>
+  <si>
+    <t>Study Institution3</t>
   </si>
 </sst>
 </file>
@@ -1118,8 +1124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C03A80-53F5-C744-BC65-FAA91BD85774}">
   <dimension ref="A1:EC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="CL1" workbookViewId="0">
+      <selection activeCell="CO4" sqref="CO4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1772,13 +1778,13 @@
         <v>197</v>
       </c>
       <c r="BL2" s="1" t="s">
-        <v>92</v>
+        <v>222</v>
       </c>
       <c r="BM2" s="1">
         <v>3013454562</v>
       </c>
       <c r="BN2" s="1" t="s">
-        <v>93</v>
+        <v>223</v>
       </c>
       <c r="BO2" s="1" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
"Made changes to Assertions
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jains18/git/CBIIT-Test-Automation/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BF6D01-92F7-7441-B9D8-D3610761C592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB28192-7FE8-FC48-AE1C-F53CF2FEB107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33960" windowHeight="16940" xr2:uid="{B3E53782-D40D-CC47-BA00-27DFD8C445AF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="FanconiScreener" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -749,12 +750,6 @@
     <t>WhatIsYourNameLastName</t>
   </si>
   <si>
-    <t>Tester-1</t>
-  </si>
-  <si>
-    <t>Tester-2</t>
-  </si>
-  <si>
     <t>WhatIsYourRelationshipToParticipant</t>
   </si>
   <si>
@@ -830,18 +825,12 @@
     <t>M-3</t>
   </si>
   <si>
-    <t>Tester-3</t>
-  </si>
-  <si>
     <t>Fanconi-4</t>
   </si>
   <si>
     <t>M-4</t>
   </si>
   <si>
-    <t>Tester-4</t>
-  </si>
-  <si>
     <t>charmsparticipant4@yopmail.com</t>
   </si>
   <si>
@@ -893,9 +882,6 @@
     <t>M-5</t>
   </si>
   <si>
-    <t>Tester-5</t>
-  </si>
-  <si>
     <t>charmsparticipant5@yopmail.com</t>
   </si>
   <si>
@@ -957,6 +943,21 @@
   </si>
   <si>
     <t>Caucasian (white), Black/African American, Native Hawaiian/Other Pacific Islander, American Indian/Alaskan Native, Asian, Other</t>
+  </si>
+  <si>
+    <t>tester-1</t>
+  </si>
+  <si>
+    <t>tester-2</t>
+  </si>
+  <si>
+    <t>tester-3</t>
+  </si>
+  <si>
+    <t>tester-4</t>
+  </si>
+  <si>
+    <t>tester-5</t>
   </si>
 </sst>
 </file>
@@ -1379,8 +1380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C03A80-53F5-C744-BC65-FAA91BD85774}">
   <dimension ref="A1:EP8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="AO3" sqref="AO3"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <selection activeCell="AH8" sqref="AH8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1485,10 +1486,10 @@
         <v>232</v>
       </c>
       <c r="K1" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>235</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>237</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>52</v>
@@ -1512,13 +1513,13 @@
         <v>10</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="U1" s="6" t="s">
         <v>11</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="W1" s="6" t="s">
         <v>53</v>
@@ -1584,7 +1585,7 @@
         <v>24</v>
       </c>
       <c r="AR1" s="6" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="AS1" s="6" t="s">
         <v>25</v>
@@ -1701,7 +1702,7 @@
         <v>28</v>
       </c>
       <c r="CE1" s="6" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="CF1" s="6" t="s">
         <v>29</v>
@@ -1716,10 +1717,10 @@
         <v>122</v>
       </c>
       <c r="CJ1" s="6" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="CK1" s="6" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="CL1" s="6" t="s">
         <v>100</v>
@@ -1773,7 +1774,7 @@
         <v>124</v>
       </c>
       <c r="DC1" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="DD1" s="6" t="s">
         <v>126</v>
@@ -1854,7 +1855,7 @@
         <v>167</v>
       </c>
       <c r="ED1" s="6" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="EE1" s="6" t="s">
         <v>169</v>
@@ -1904,7 +1905,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>233</v>
+        <v>298</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>3</v>
@@ -1994,7 +1995,7 @@
         <v>58</v>
       </c>
       <c r="AR2" s="1" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="AS2" s="1" t="s">
         <v>3</v>
@@ -2290,7 +2291,7 @@
         <v>225</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>234</v>
+        <v>299</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>229</v>
@@ -2308,25 +2309,25 @@
         <v>17644</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>229</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="AD3" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="AE3" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="AF3" s="1">
         <v>3015774089</v>
@@ -2341,10 +2342,10 @@
         <v>3015567865</v>
       </c>
       <c r="AJ3" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="AK3" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="AS3" s="1" t="s">
         <v>229</v>
@@ -2353,7 +2354,7 @@
         <v>3</v>
       </c>
       <c r="CA3" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="CB3" s="4">
         <v>40128</v>
@@ -2362,40 +2363,40 @@
         <v>3</v>
       </c>
       <c r="CD3" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="CF3" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="CG3" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="CF3" s="1" t="s">
+      <c r="CH3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="CI3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="CL3" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="CG3" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="CH3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="CI3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="CL3" s="1" t="s">
-        <v>248</v>
       </c>
       <c r="CM3" s="1" t="s">
         <v>108</v>
       </c>
       <c r="CN3" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="CO3" s="1" t="s">
         <v>107</v>
       </c>
       <c r="CP3" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="CQ3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="CR3" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="CS3" s="1" t="s">
         <v>3</v>
@@ -2437,19 +2438,19 @@
         <v>97</v>
       </c>
       <c r="DK3" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="DL3" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="DM3" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="DL3" s="1" t="s">
+      <c r="DN3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="DO3" s="1" t="s">
         <v>252</v>
-      </c>
-      <c r="DM3" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="DN3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="DO3" s="1" t="s">
-        <v>254</v>
       </c>
       <c r="DP3" s="1" t="s">
         <v>146</v>
@@ -2476,10 +2477,10 @@
         <v>160</v>
       </c>
       <c r="DZ3" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="EB3" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="EE3" s="1" t="s">
         <v>170</v>
@@ -2523,16 +2524,16 @@
         <v>54</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>260</v>
+        <v>300</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="N4" s="1">
         <v>1948</v>
@@ -2547,25 +2548,25 @@
         <v>17644</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="AD4" s="5" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="AE4" s="5" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="AF4" s="1">
         <v>3015774089</v>
@@ -2580,32 +2581,32 @@
         <v>3015567865</v>
       </c>
       <c r="AJ4" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="AK4" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="AS4" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="BZ4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="CA4" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="CB4" s="4"/>
       <c r="CC4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="CD4" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="CF4" s="1" t="s">
         <v>97</v>
       </c>
       <c r="CG4" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="CH4" s="1" t="s">
         <v>3</v>
@@ -2614,34 +2615,34 @@
         <v>3</v>
       </c>
       <c r="CL4" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="CM4" s="1" t="s">
         <v>108</v>
       </c>
       <c r="CN4" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="CO4" s="1" t="s">
         <v>107</v>
       </c>
       <c r="CP4" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="CQ4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="CR4" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="CS4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="CT4" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="CX4" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="CY4" s="1" t="s">
         <v>119</v>
@@ -2653,7 +2654,7 @@
         <v>3</v>
       </c>
       <c r="DB4" s="6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="DC4" s="4"/>
       <c r="DE4" s="1" t="s">
@@ -2663,28 +2664,28 @@
         <v>130</v>
       </c>
       <c r="DG4" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="DK4" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="DL4" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="DM4" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="DN4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="DO4" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="DP4" s="1" t="s">
         <v>146</v>
       </c>
       <c r="DQ4" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="DU4" s="1" t="s">
         <v>229</v>
@@ -2705,10 +2706,10 @@
         <v>162</v>
       </c>
       <c r="EA4" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="EB4" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="EE4" s="1" t="s">
         <v>170</v>
@@ -2752,13 +2753,13 @@
         <v>54</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>263</v>
+        <v>301</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>3</v>
@@ -2776,31 +2777,31 @@
         <v>17644</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>229</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="AD5" s="5" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="AE5" s="1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="AF5" s="1">
         <v>3015774089</v>
@@ -2815,7 +2816,7 @@
         <v>3015567865</v>
       </c>
       <c r="AJ5" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="AK5" s="1" t="s">
         <v>39</v>
@@ -2953,10 +2954,10 @@
         <v>45</v>
       </c>
       <c r="CE5" s="1" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="CF5" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="CG5" s="1" t="s">
         <v>99</v>
@@ -2982,7 +2983,7 @@
         <v>3</v>
       </c>
       <c r="DO5" s="1" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="DP5" s="1" t="s">
         <v>146</v>
@@ -2991,7 +2992,7 @@
         <v>121</v>
       </c>
       <c r="DR5" s="1" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="DS5" s="1">
         <v>1967</v>
@@ -3021,7 +3022,7 @@
         <v>51</v>
       </c>
       <c r="ED5" s="1" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="EE5" s="1" t="s">
         <v>170</v>
@@ -3065,13 +3066,13 @@
         <v>54</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>281</v>
+        <v>302</v>
       </c>
       <c r="Q6" s="4"/>
       <c r="AD6" s="5"/>
@@ -3091,7 +3092,7 @@
         <v>227</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>224</v>
@@ -3100,10 +3101,10 @@
         <v>225</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>236</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>3</v>
@@ -3124,7 +3125,7 @@
         <v>17644</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>3</v>
@@ -3148,10 +3149,10 @@
         <v>20147</v>
       </c>
       <c r="AD7" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="AE7" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="AF7" s="1">
         <v>3015774089</v>
@@ -3166,7 +3167,7 @@
         <v>3014524258</v>
       </c>
       <c r="AJ7" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="AK7" s="1" t="s">
         <v>39</v>
@@ -3400,7 +3401,7 @@
         <v>144</v>
       </c>
       <c r="DP7" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="DQ7" s="1" t="s">
         <v>121</v>
@@ -3480,22 +3481,22 @@
         <v>223</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>228</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>281</v>
+        <v>302</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>136</v>
@@ -3525,13 +3526,13 @@
         <v>229</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="AD8" s="5" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="AE8" s="1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -3551,6 +3552,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEEF0C7A-1495-D84C-AF4F-5830779442F6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0099EE8B-FA58-9042-B22E-97A35F4834AD}">
   <dimension ref="C2:F16"/>
   <sheetViews>

</xml_diff>